<commit_message>
code merge from review(enterprise) branch for sprint 6 tasks
git-svn-id: http://svn.enterpi.com/repos/Mintmesh_enterprise/trunk@10354 2a077918-f434-4ae4-a93c-d96c61136af1
</commit_message>
<xml_diff>
--- a/public/downloads/sample_template.xlsx
+++ b/public/downloads/sample_template.xlsx
@@ -40,10 +40,10 @@
     <t>Status</t>
   </si>
   <si>
+    <t>OPTIONAL</t>
+  </si>
+  <si>
     <t>REQUIRED</t>
-  </si>
-  <si>
-    <t>OPTIONAL</t>
   </si>
 </sst>
 </file>
@@ -53,7 +53,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -83,12 +83,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -133,16 +127,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -226,12 +216,12 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="G5" activeCellId="0" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.5148148148148"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.6"/>
     <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="10.4518518518519"/>
   </cols>
   <sheetData>
@@ -256,23 +246,23 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="0" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C2" s="0" t="s">
         <v>6</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>